<commit_message>
added new FAN_ENABLE output
</commit_message>
<xml_diff>
--- a/CPRacing Designs/Control Board/mcu_pinouts.xlsx
+++ b/CPRacing Designs/Control Board/mcu_pinouts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\OneDrive\Documents\GitHub\Altium-Designs\CPRacing Designs\Control Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78C64C3-FDB4-4EF6-A49B-B5052C5071C5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72B2A3F-30A0-479F-A82E-F9719F3B7816}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7470" xr2:uid="{F052E91A-9F3B-4B42-9C56-09703667230C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="81">
   <si>
     <t>input</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>PTC9</t>
+  </si>
+  <si>
+    <t>FAN_ENABLE</t>
+  </si>
+  <si>
+    <t>PTD2</t>
   </si>
 </sst>
 </file>
@@ -618,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC69746-96CB-4621-91D7-981EF49FF841}">
-  <dimension ref="B2:M28"/>
+  <dimension ref="B2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -843,6 +849,21 @@
       <c r="F8">
         <v>49</v>
       </c>
+      <c r="H8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
       <c r="M8" t="s">
         <v>27</v>
       </c>
@@ -863,6 +884,21 @@
       <c r="F9">
         <v>5</v>
       </c>
+      <c r="H9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
       <c r="M9" t="s">
         <v>28</v>
       </c>
@@ -883,6 +919,21 @@
       <c r="F10">
         <v>6</v>
       </c>
+      <c r="H10" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>46</v>
+      </c>
       <c r="M10" t="s">
         <v>74</v>
       </c>
@@ -1059,137 +1110,103 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23">
-        <v>3</v>
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
+        <v>55</v>
       </c>
       <c r="F23">
-        <v>51</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24">
-        <v>3</v>
+        <v>60</v>
+      </c>
+      <c r="E24" t="s">
+        <v>55</v>
       </c>
       <c r="F24">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
         <v>55</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E26" t="s">
         <v>55</v>
       </c>
       <c r="F26">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tweaked to fix design rules errors
</commit_message>
<xml_diff>
--- a/CPRacing Designs/Control Board/mcu_pinouts.xlsx
+++ b/CPRacing Designs/Control Board/mcu_pinouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\OneDrive\Documents\GitHub\Altium-Designs\CPRacing Designs\Control Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D1A56C-9CD1-4C82-9DA2-E5149919FF56}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CF5BE6-7D4E-4C8F-BBCF-658F32E6F167}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7470" xr2:uid="{F052E91A-9F3B-4B42-9C56-09703667230C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="78">
   <si>
     <t>input</t>
   </si>
@@ -261,13 +261,16 @@
   </si>
   <si>
     <t>PTB13</t>
+  </si>
+  <si>
+    <t>*NEED UPDATE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,8 +278,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +305,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -308,11 +324,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,7 +647,7 @@
   <dimension ref="B2:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -640,7 +657,7 @@
     <col min="4" max="4" width="10.6328125" customWidth="1"/>
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
     <col min="6" max="6" width="7.6328125" customWidth="1"/>
-    <col min="8" max="8" width="21.26953125" customWidth="1"/>
+    <col min="8" max="8" width="25.08984375" customWidth="1"/>
     <col min="10" max="10" width="11.453125" customWidth="1"/>
     <col min="11" max="11" width="10.6328125" customWidth="1"/>
   </cols>
@@ -991,7 +1008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" ht="26" x14ac:dyDescent="0.6">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1003,6 +1020,9 @@
       </c>
       <c r="F16">
         <v>12</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
@@ -1117,5 +1137,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>